<commit_message>
assets toegevoegd naam veranderd en ico erbij
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Logboek</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>PyramidPanic</t>
+  </si>
+  <si>
+    <t>Het spel PyramidPanic gespeeld.</t>
+  </si>
+  <si>
+    <t>Ico toe gevoegd. Naam in PyramidPanic gemaakt. En assets toegevoegd aan game</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,30 +572,42 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="C8" s="10">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E8" s="9">
         <v>2</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="10">
         <f t="shared" ref="G8:G12" si="0">D8-C8</f>
-        <v>0</v>
+        <v>1.7361111111111105E-2</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.4284722222222222</v>
+      </c>
       <c r="E9" s="9">
         <v>3</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1805555555555514E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -790,7 +808,7 @@
       </c>
       <c r="G26" s="10">
         <f>SUM(G7:G22)</f>
-        <v>3.4722222222222265E-2</v>
+        <v>6.3888888888888884E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1011,7 +1029,7 @@
       </c>
       <c r="B7" s="4">
         <f>'weeknr 45'!G26</f>
-        <v>3.4722222222222265E-2</v>
+        <v>6.3888888888888884E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
@@ -1026,7 +1044,7 @@
       </c>
       <c r="B9" s="4">
         <f>SUM(B7:B8)</f>
-        <v>3.4722222222222265E-2</v>
+        <v>6.3888888888888884E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MouseVisible en escape toegevoegd
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555"/>
   </bookViews>
   <sheets>
-    <sheet name="weeknr 45" sheetId="1" r:id="rId1"/>
-    <sheet name="week 46" sheetId="2" r:id="rId2"/>
+    <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
+    <sheet name="week 49" sheetId="2" r:id="rId2"/>
     <sheet name="Totaal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Logboek</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Ico toe gevoegd. Naam in PyramidPanic gemaakt. En assets toegevoegd aan game</t>
+  </si>
+  <si>
+    <t>Alle essets geordend en github + logboek bijgewerkt.</t>
+  </si>
+  <si>
+    <t>Spritebatch toegevoegd voor background.</t>
+  </si>
+  <si>
+    <t>IsMouseVisble = true gemaakt en escape toegevoegd.</t>
   </si>
 </sst>
 </file>
@@ -477,7 +486,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,45 +623,63 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.4513888888888889</v>
+      </c>
       <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="G10" s="10">
         <f t="shared" ref="G10:G11" si="1">D10-C10</f>
-        <v>0</v>
+        <v>1.3888888888888895E-2</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="10">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.46527777777777773</v>
+      </c>
       <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="G11" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="10">
+        <v>0.46875</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="E12" s="9">
         <v>6</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7361111111111105E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,7 +835,7 @@
       </c>
       <c r="G26" s="10">
         <f>SUM(G7:G22)</f>
-        <v>6.3888888888888884E-2</v>
+        <v>0.10555555555555551</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +997,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1025,11 +1052,11 @@
     </row>
     <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" s="4">
-        <f>'weeknr 45'!G26</f>
-        <v>6.3888888888888884E-2</v>
+        <f>'weeknr 48'!G26</f>
+        <v>0.10555555555555551</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
@@ -1044,7 +1071,7 @@
       </c>
       <c r="B9" s="4">
         <f>SUM(B7:B8)</f>
-        <v>6.3888888888888884E-2</v>
+        <v>0.10555555555555551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
StartScene bij gewerkt alleen nog bugs uit halen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Logboek</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Rest van de scenes gemaakt.</t>
+  </si>
+  <si>
+    <t>Scene waardes ingevuld. Moeten nog wat fouten uitgehaald worden.</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,16 +757,22 @@
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="10">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.59375</v>
+      </c>
       <c r="E17" s="9">
         <v>10</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G17" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -862,7 +871,7 @@
       </c>
       <c r="G26" s="10">
         <f>SUM(G7:G22)</f>
-        <v>0.18194444444444441</v>
+        <v>0.20277777777777778</v>
       </c>
     </row>
   </sheetData>
@@ -1083,7 +1092,7 @@
       </c>
       <c r="B7" s="4">
         <f>'weeknr 48'!G26</f>
-        <v>0.18194444444444441</v>
+        <v>0.20277777777777778</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
@@ -1098,7 +1107,7 @@
       </c>
       <c r="B9" s="4">
         <f>SUM(B7:B8)</f>
-        <v>0.18194444444444441</v>
+        <v>0.20277777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scene's gemaakt en en PlayScene en Start Scene in PyramidPanic gezet
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\Visual Studio 2010\Projects\school\blok2\project2\PyramidPanic\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
     <sheet name="week 49" sheetId="2" r:id="rId2"/>
     <sheet name="Totaal" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Logboek</t>
   </si>
@@ -54,18 +59,9 @@
     <t>Aplicatie/mediadev.</t>
   </si>
   <si>
-    <t>Jumbo arcade game.</t>
-  </si>
-  <si>
     <t>Jason Binneveld.</t>
   </si>
   <si>
-    <t>Maandag</t>
-  </si>
-  <si>
-    <t>Format van het standaard logboek gemaakt</t>
-  </si>
-  <si>
     <t>Weeknr:</t>
   </si>
   <si>
@@ -106,6 +102,15 @@
   </si>
   <si>
     <t>Scene waardes ingevuld. Moeten nog wat fouten uitgehaald worden.</t>
+  </si>
+  <si>
+    <t>Donderdag</t>
+  </si>
+  <si>
+    <t>StartScene in PyramaidPanic gezet</t>
+  </si>
+  <si>
+    <t>De rest van de Scene's gemaakt</t>
   </si>
 </sst>
 </file>
@@ -115,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +209,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -251,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,43 +505,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="2"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.75" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -541,7 +549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -565,9 +573,9 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.5">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5">
         <v>41637</v>
@@ -582,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7" s="10">
         <f>D7-C7</f>
@@ -590,7 +598,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="10">
@@ -603,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" ref="G8:G12" si="0">D8-C8</f>
@@ -611,7 +619,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="10">
@@ -624,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
@@ -632,7 +640,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="10">
@@ -645,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" ref="G10:G11" si="1">D10-C10</f>
@@ -653,7 +661,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="10">
@@ -666,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="1"/>
@@ -674,7 +682,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="10">
@@ -687,14 +695,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>1.7361111111111105E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="10">
@@ -707,14 +715,14 @@
         <v>7</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" ref="G13:G18" si="2">D13-C13</f>
+        <f t="shared" ref="G13:G17" si="2">D13-C13</f>
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="C14" s="10">
         <v>0.50694444444444442</v>
       </c>
@@ -725,14 +733,14 @@
         <v>8</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G14" s="10">
         <f t="shared" si="2"/>
         <v>1.736111111111116E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="C15" s="10">
         <v>0.52430555555555558</v>
       </c>
@@ -743,21 +751,21 @@
         <v>9</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G15" s="10">
         <f t="shared" si="2"/>
         <v>4.8611111111111049E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="9"/>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="28.5">
       <c r="C17" s="10">
         <v>0.57291666666666663</v>
       </c>
@@ -768,101 +776,65 @@
         <v>10</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" si="2"/>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="9">
-        <v>11</v>
-      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="10"/>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20" s="12"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="9">
-        <v>12</v>
-      </c>
+      <c r="E20" s="9"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="10">
-        <f t="shared" ref="G20:G25" si="3">D20-C20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="2:7">
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="9">
-        <v>13</v>
-      </c>
+      <c r="E21" s="9"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="9">
-        <v>14</v>
-      </c>
+      <c r="E22" s="9"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="2:7">
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="2:7">
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="9"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="2:7">
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="9"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="2:7">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
@@ -884,17 +856,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="8.85546875" style="3"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,29 +874,29 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -935,12 +907,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -963,12 +935,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B7" s="5">
-        <v>41582</v>
+        <v>41612</v>
       </c>
       <c r="C7" s="4">
         <v>0.36458333333333331</v>
@@ -980,21 +952,31 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4">
+        <f>D7-C7</f>
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="4">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1002,7 +984,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1010,7 +992,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1036,39 +1018,39 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1078,15 +1060,15 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3">
         <v>48</v>
       </c>
@@ -1095,13 +1077,13 @@
         <v>0.20277777777777778</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>46</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
propeties Scene's em Inpput begonnen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Logboek</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">IGameState gemaakt </t>
+  </si>
+  <si>
+    <t>Propeties gemaakt van gameScene's. Fout uit code Gehaald en begonnen aan Input.cs</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1028,12 +1031,21 @@
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="4">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.53125</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1109,7 +1121,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>8.680555555555558E-2</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bijgewerkt tot waar de leraar is
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
     <sheet name="week 49" sheetId="2" r:id="rId2"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId3"/>
+    <sheet name="week 50" sheetId="4" r:id="rId3"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>Logboek</t>
   </si>
@@ -120,6 +121,9 @@
   </si>
   <si>
     <t>Propeties gemaakt van gameScene's. Fout uit code Gehaald en begonnen aan Input.cs</t>
+  </si>
+  <si>
+    <t>Alles bijgewerkt naar commit leraar</t>
   </si>
 </sst>
 </file>
@@ -865,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1131,10 +1135,254 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41620</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4">
+        <f>D7-C7</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G16" si="0">D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <f>SUM(G7:G17)</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1198,17 +1446,29 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3">
-        <v>46</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="B8" s="4">
+        <f>'week 49'!G18</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="3">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4">
+        <f>'week 50'!G18</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <f>SUM(B7:B8)</f>
-        <v>0.20277777777777778</v>
+        <v>0.32777777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backgroud toegevoeg startscene en title begin aan gemaakt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Logboek</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Alles bijgewerkt naar commit leraar</t>
+  </si>
+  <si>
+    <t>StartScene achtergrond toegevoegd en begin gemaakt aan title</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1141,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1229,10 +1232,10 @@
       <c r="D7" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="9">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="4">
@@ -1240,18 +1243,24 @@
         <v>1.3888888888888951E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="28.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3">
+      <c r="C8" s="10">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="E8" s="9">
         <v>2</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="G8" s="4">
         <f t="shared" ref="G8:G16" si="0">D8-C8</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1259,10 +1268,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3">
+      <c r="E9" s="9">
         <v>3</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1273,10 +1282,10 @@
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="3">
+      <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1287,10 +1296,10 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="3">
+      <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1301,7 +1310,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1312,7 +1321,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1323,7 +1332,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1334,7 +1343,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1345,7 +1354,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1356,7 +1365,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
@@ -1369,11 +1378,12 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>1.3888888888888951E-2</v>
+        <v>5.208333333333337E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1459,7 +1469,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>1.3888888888888951E-2</v>
+        <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
De title in StartScene toegevoegd
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Logboek</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>StartScene achtergrond toegevoegd en begin gemaakt aan title</t>
+  </si>
+  <si>
+    <t>De Title in StartScene gezet</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1144,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1266,15 +1269,21 @@
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="E9" s="9">
         <v>3</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666685E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1378,7 +1387,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>5.208333333333337E-2</v>
+        <v>6.2500000000000056E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1478,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>5.208333333333337E-2</v>
+        <v>6.2500000000000056E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
Menu class aangemaakt en eerste button waar gemaakt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Logboek</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>De Title in StartScene gezet</t>
+  </si>
+  <si>
+    <t>Menu class aangemaakt en eerst button aangemaakt.</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -217,6 +220,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1241,7 +1247,7 @@
       <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="10">
         <f>D7-C7</f>
         <v>1.3888888888888951E-2</v>
       </c>
@@ -1261,7 +1267,7 @@
       <c r="F8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="10">
         <f t="shared" ref="G8:G16" si="0">D8-C8</f>
         <v>3.819444444444442E-2</v>
       </c>
@@ -1281,35 +1287,41 @@
       <c r="F9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="28.5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="10">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="9">
         <v>5</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="4">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1317,10 +1329,10 @@
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="4">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1328,10 +1340,10 @@
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="4">
+      <c r="G13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1339,10 +1351,10 @@
     <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="4">
+      <c r="G14" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1350,10 +1362,10 @@
     <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="4">
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1361,10 +1373,10 @@
     <row r="16" spans="1:7">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="4">
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1372,23 +1384,27 @@
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="F18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>6.2500000000000056E-2</v>
-      </c>
+        <v>9.3750000000000056E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1478,7 +1494,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>6.2500000000000056E-2</v>
+        <v>9.3750000000000056E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
De buttons aan StartScene toegevoegd
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Logboek</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Menu class aangemaakt en eerst button aangemaakt.</t>
+  </si>
+  <si>
+    <t>Alle buttons aangemaakt en gedrawed op het StartScene.</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1153,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1312,18 +1315,24 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="28.5">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.50347222222222221</v>
+      </c>
       <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4305555555555525E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1399,7 +1408,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>9.3750000000000056E-2</v>
+        <v>0.11805555555555558</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1494,7 +1503,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>9.3750000000000056E-2</v>
+        <v>0.11805555555555558</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
Buttons in de List<Image> toegevoegd
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Logboek</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Alle buttons aangemaakt en gedrawed op het StartScene.</t>
+  </si>
+  <si>
+    <t>De buttons in een List&lt;Image&gt; toegevoegd</t>
   </si>
 </sst>
 </file>
@@ -1338,12 +1341,21 @@
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="F12" s="8"/>
+      <c r="C12" s="10">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666741E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1408,7 +1420,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>0.11805555555555558</v>
+        <v>0.12847222222222232</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1503,7 +1515,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>0.11805555555555558</v>
+        <v>0.12847222222222232</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
Knoppen werkend gemaakt door middel van edgedetection en begin gemaakt om door middel van enter naar de juiste scene te gaan
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Logboek</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>De buttons in een List&lt;Image&gt; toegevoegd</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Knoppen werkend gemaakt met edge detection. Begin gemaakt aan Scene's dat als je enter drukt naar de juiste scene gaat.</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1162,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1361,23 +1367,41 @@
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="F13" s="8"/>
+      <c r="C13" s="10">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.53125</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>1.7361111111111049E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="42.75">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="F14" s="8"/>
+      <c r="C14" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="G14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1420,7 +1444,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>0.12847222222222232</v>
+        <v>0.19791666666666674</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1515,7 +1539,7 @@
       </c>
       <c r="B9" s="4">
         <f>'week 50'!G18</f>
-        <v>0.12847222222222232</v>
+        <v>0.19791666666666674</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>

<commit_message>
Fout in menu gefixt 2 Scene aangemaakt en b toets terug van elke Scene
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
     <sheet name="week 49" sheetId="2" r:id="rId2"/>
     <sheet name="week 50" sheetId="4" r:id="rId3"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId4"/>
+    <sheet name="week 2" sheetId="6" r:id="rId4"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
   <si>
     <t>Logboek</t>
   </si>
@@ -145,6 +146,9 @@
   </si>
   <si>
     <t>Knoppen werkend gemaakt met edge detection. Begin gemaakt aan Scene's dat als je enter drukt naar de juiste scene gaat.</t>
+  </si>
+  <si>
+    <t>Menu Gemaakt, hij ging uit het beeld. scoreScene en LoadScene aangemaakt en van elke scene kan je terug via b</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1459,10 +1463,268 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42.75">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41648</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="10">
+        <f>D7-C7</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10">
+        <f t="shared" ref="G8:G16" si="0">D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="9">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="3">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="3">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <f>SUM(G7:G17)</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1543,15 +1805,25 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4">
+        <f>'week 2'!G18</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <f>SUM(B7:B8)</f>
         <v>0.32777777777777778</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Restante van Scene's toegevoegd
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>Logboek</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Menu Gemaakt, hij ging uit het beeld. scoreScene en LoadScene aangemaakt en van elke scene kan je terug via b</t>
+  </si>
+  <si>
+    <t>In PyramidPanic de Scenes toegevoegd</t>
   </si>
 </sst>
 </file>
@@ -1466,7 +1469,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1571,15 +1574,21 @@
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="C8" s="10">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="E8" s="9">
         <v>2</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G8" s="10">
         <f t="shared" ref="G8:G16" si="0">D8-C8</f>
-        <v>0</v>
+        <v>1.3888888888888895E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1706,7 +1715,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>1.7361111111111105E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1810,7 +1819,7 @@
       </c>
       <c r="B10" s="4">
         <f>'week 2'!G18</f>
-        <v>1.7361111111111105E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
Mouse toegevoegd en begin rectangle
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t>Logboek</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>End Scene Afgemaakt en bij de menu goed neer gezet</t>
+  </si>
+  <si>
+    <t>Begin mouse gemaakt en rectangle aangemaakt.</t>
   </si>
 </sst>
 </file>
@@ -1614,18 +1617,24 @@
         <v>1.3888888888888951E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="28.5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="10">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1724,7 +1733,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>4.5138888888888951E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1828,7 +1837,7 @@
       </c>
       <c r="B10" s="4">
         <f>'week 2'!G18</f>
-        <v>4.5138888888888951E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
Eerste knop help werkend gemaakt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t>Logboek</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Begin mouse gemaakt en rectangle aangemaakt.</t>
+  </si>
+  <si>
+    <t>MouseRect in draw aangemaakt</t>
+  </si>
+  <si>
+    <t>Eerste knop werkend gemaakt met muis</t>
   </si>
 </sst>
 </file>
@@ -1475,7 +1481,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1640,29 +1646,41 @@
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666685E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="10">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="E12" s="3">
         <v>6</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4305555555555525E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1733,7 +1751,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>6.25E-2</v>
+        <v>9.722222222222221E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1837,7 +1855,7 @@
       </c>
       <c r="B10" s="4">
         <f>'week 2'!G18</f>
-        <v>6.25E-2</v>
+        <v>9.722222222222221E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
Alle knoppen werkend gemaakt doormiddel van de muis
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>Logboek</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Eerste knop werkend gemaakt met muis</t>
+  </si>
+  <si>
+    <t>Alle knoppen werkend gemaakt doormiddel van de muis</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1484,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1683,18 +1686,24 @@
         <v>2.4305555555555525E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="28.5">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="10">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="E13" s="3">
         <v>7</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444753E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1751,7 +1760,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>9.722222222222221E-2</v>
+        <v>0.10416666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1855,7 +1864,7 @@
       </c>
       <c r="B10" s="4">
         <f>'week 2'!G18</f>
-        <v>9.722222222222221E-2</v>
+        <v>0.10416666666666669</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
Helpmethod gemaakt voor mouse detection
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>Logboek</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Alle knoppen werkend gemaakt doormiddel van de muis</t>
+  </si>
+  <si>
+    <t>Help Method gemaakt voor Mouse Detection</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1487,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1709,15 +1712,21 @@
     <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="10">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="3">
         <v>8</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="G14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7361111111111105E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1760,7 +1769,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>0.10416666666666669</v>
+        <v>0.12152777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1864,7 +1873,7 @@
       </c>
       <c r="B10" s="4">
         <f>'week 2'!G18</f>
-        <v>0.10416666666666669</v>
+        <v>0.12152777777777779</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
beetle.cs en ibeetlestate.cs aangemaakt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
     <sheet name="week 49" sheetId="2" r:id="rId2"/>
     <sheet name="week 50" sheetId="4" r:id="rId3"/>
     <sheet name="week 2" sheetId="6" r:id="rId4"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId5"/>
+    <sheet name="week 3" sheetId="7" r:id="rId5"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
   <si>
     <t>Logboek</t>
   </si>
@@ -170,6 +171,12 @@
   </si>
   <si>
     <t>Help Method gemaakt voor Mouse Detection</t>
+  </si>
+  <si>
+    <t>Woensdag</t>
+  </si>
+  <si>
+    <t>beetle.cs en ibeetlestate.cs aangemaakt</t>
   </si>
 </sst>
 </file>
@@ -223,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -260,6 +267,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1486,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1784,10 +1794,251 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="15">
+        <v>41661</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="10">
+        <f>D7-C7</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10">
+        <f t="shared" ref="G8:G16" si="0">D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <f>SUM(G7:G17)</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1877,10 +2128,19 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4">
+        <f>'week 3'!G18</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="4">
         <f>SUM(B7:B8)</f>
         <v>0.32777777777777778</v>
       </c>

</xml_diff>

<commit_message>
Beetle class ingevuld en iBeetleClass ingevuld. WalkUp en WalkDOwn gemaakt voor beetle
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>Logboek</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>beetle.cs en ibeetlestate.cs aangemaakt</t>
+  </si>
+  <si>
+    <t>Beetle class ingevuld en iBeetleClass ingevuld. WalkUp en WalkDOwn gemaakt voor beetle</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1800,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1899,16 +1902,24 @@
         <v>4.8611111111110938E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="42.75">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="10">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="G8" s="10">
         <f t="shared" ref="G8:G16" si="0">D8-C8</f>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2020,7 +2031,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>4.8611111111110938E-3</v>
+        <v>2.2222222222222143E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2133,7 +2144,7 @@
       </c>
       <c r="B11" s="4">
         <f>'week 3'!G18</f>
-        <v>4.8611111111110938E-3</v>
+        <v>2.2222222222222143E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
AnimatedSprite gemaakt en bij up en down bij gewerkt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
   <si>
     <t>Logboek</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Beetle class ingevuld en iBeetleClass ingevuld. WalkUp en WalkDOwn gemaakt voor beetle</t>
+  </si>
+  <si>
+    <t>AnimatedSprite gemaakt en bij up en down bij gewerkt</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1803,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1922,16 +1925,24 @@
         <v>1.7361111111111049E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="28.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="4">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.736111111111116E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2031,7 +2042,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>2.2222222222222143E-2</v>
+        <v>3.9583333333333304E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2144,7 +2155,7 @@
       </c>
       <c r="B11" s="4">
         <f>'week 3'!G18</f>
-        <v>2.2222222222222143E-2</v>
+        <v>3.9583333333333304E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
scorpion laten draaien en bugs eruit
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
   <si>
     <t>Logboek</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Scorpion gemaakt </t>
+  </si>
+  <si>
+    <t>De scorpion laten draaien en foute eruit gehaald.</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1809,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1968,16 +1971,28 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
+    <row r="11" spans="1:7" ht="28.5">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="15">
+        <v>41662</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.6388888888888962E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2053,7 +2068,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>6.0416666666666674E-2</v>
+        <v>8.6805555555555636E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2166,7 +2181,7 @@
       </c>
       <c r="B11" s="4">
         <f>'week 3'!G18</f>
-        <v>6.0416666666666674E-2</v>
+        <v>8.6805555555555636E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
explorer klan van links e recht lopen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <t>Logboek</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>IEntityState in plaats van IbeetleState en IScorpionState</t>
+  </si>
+  <si>
+    <t>bezig met explorer</t>
+  </si>
+  <si>
+    <t>Explorer kan nu van links en recht lopen</t>
   </si>
 </sst>
 </file>
@@ -1812,7 +1818,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F13:F14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2021,23 +2027,41 @@
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="F13" s="8"/>
+      <c r="C13" s="10">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.53125</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1076388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="F14" s="8"/>
+      <c r="C14" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="G14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2080,7 +2104,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>0.11111111111111116</v>
+        <v>0.23958333333333343</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2193,7 +2217,7 @@
       </c>
       <c r="B11" s="4">
         <f>'week 3'!G18</f>
-        <v>0.11111111111111116</v>
+        <v>0.23958333333333343</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
Comentaar bij tekst gezet en ExplorerWalkUp gemaakt
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 48" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,15 @@
     <sheet name="week 50" sheetId="4" r:id="rId3"/>
     <sheet name="week 2" sheetId="6" r:id="rId4"/>
     <sheet name="week 3" sheetId="7" r:id="rId5"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId6"/>
+    <sheet name="week 4" sheetId="8" r:id="rId6"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
   <si>
     <t>Logboek</t>
   </si>
@@ -198,6 +199,9 @@
   </si>
   <si>
     <t>Explorer kan nu van links en recht lopen</t>
+  </si>
+  <si>
+    <t>Comentaar bij tekst gezet en ExplorerWalkUp gemaakt</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2118,6 +2122,247 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.5">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="15">
+        <v>41669</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="10">
+        <f>D7-C7</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10">
+        <f t="shared" ref="G8:G16" si="0">D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <f>SUM(G7:G17)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Gewerkt aan ExplorerIdleWalk En collisen geven dat de explorer niet uit he tbeeld kan lopen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>Logboek</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Vector2 pivot en rotatie veranderd in beetle en scorpion</t>
+  </si>
+  <si>
+    <t>Gewerkt aan ExplorerIdleWalk En collisen geven dat de explorer niet uit he tbeeld kan lopen</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2132,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2251,16 +2254,24 @@
         <v>3.4722222222222654E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="42.75">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2360,7 +2371,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>3.4722222222222265E-2</v>
+        <v>8.6805555555555636E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>

<commit_message>
Explorer kan niet meer uit het scherm lopen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="62">
   <si>
     <t>Logboek</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Gewerkt aan ExplorerIdleWalk En collisen geven dat de explorer niet uit he tbeeld kan lopen</t>
+  </si>
+  <si>
+    <t>Comentaar neergezet en up gefixt</t>
   </si>
 </sst>
 </file>
@@ -2132,7 +2135,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2277,13 +2280,21 @@
     <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
+      <c r="C10" s="10">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E10" s="9">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4305555555555636E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2371,7 +2382,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>8.6805555555555636E-2</v>
+        <v>0.11111111111111127</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>

<commit_message>
scorpion kan zijn grensen aangrijpen
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
   <si>
     <t>Logboek</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>treasure toegevoegd</t>
+  </si>
+  <si>
+    <t>scorpion kan zijn grensen aangrijpen</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2421,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,15 +2547,21 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.39999999999999997</v>
+      </c>
       <c r="E9" s="9">
         <v>3</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2656,7 +2665,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>2.1527777777777757E-2</v>
+        <v>3.1944444444444386E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bezig met beetle en scorpion draaien
</commit_message>
<xml_diff>
--- a/PyramidPanic.xlsx
+++ b/PyramidPanic.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
   <si>
     <t>Logboek</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>scorpion kan zijn grensen aangrijpen</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>Bezig met draaien van scorpion en beetle</t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2427,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,32 +2570,44 @@
         <v>1.041666666666663E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="10">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7083333333333348E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.46180555555555558</v>
+      </c>
       <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,7 +2683,7 @@
       </c>
       <c r="G18" s="4">
         <f>SUM(G7:G17)</f>
-        <v>3.1944444444444386E-2</v>
+        <v>7.9861111111111049E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>